<commit_message>
avg_dev subtract from estimate + plot
</commit_message>
<xml_diff>
--- a/seacreatures.xlsx
+++ b/seacreatures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bd2799b14fed3a1/Onenote/GitHub/fish_species_detection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaspe\OneDrive\Onenote\GitHub\fish_species_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="380" documentId="11_960DBF7531BD0F2A2F3CF188BD7C7455F3707528" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32B5925A-7983-4D55-A39F-691AED661569}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB83E26-7CB7-478E-8E74-B4A6425D2B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1695" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L270"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2">
-        <v>1</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,9 @@
         <v>28</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="D71" s="2">
+        <v>148</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
@@ -1626,7 +1628,9 @@
         <v>22.5</v>
       </c>
       <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="D72" s="2">
+        <v>150</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
@@ -1636,7 +1640,9 @@
         <v>26.5</v>
       </c>
       <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="D73" s="2">
+        <v>152</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
@@ -1646,7 +1652,9 @@
         <v>21.5</v>
       </c>
       <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="D74" s="2">
+        <v>154</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
@@ -1656,7 +1664,9 @@
         <v>24.5</v>
       </c>
       <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="D75" s="2">
+        <v>156</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
@@ -1666,7 +1676,9 @@
         <v>29.5</v>
       </c>
       <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="D76" s="2">
+        <v>158</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
@@ -1676,7 +1688,9 @@
         <v>27.5</v>
       </c>
       <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="D77" s="2">
+        <v>160</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
@@ -1686,7 +1700,9 @@
         <v>25</v>
       </c>
       <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="D78" s="2">
+        <v>162</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
@@ -1696,7 +1712,9 @@
         <v>27</v>
       </c>
       <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="D79" s="2">
+        <v>164</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
@@ -1706,7 +1724,9 @@
         <v>26.5</v>
       </c>
       <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="D80" s="2">
+        <v>166</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
@@ -1716,7 +1736,9 @@
         <v>20.5</v>
       </c>
       <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2">
+        <v>168</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
@@ -1726,7 +1748,9 @@
         <v>28.5</v>
       </c>
       <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2">
+        <v>170</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
@@ -1736,7 +1760,9 @@
         <v>26</v>
       </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="D83" s="2">
+        <v>172</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
@@ -1746,7 +1772,9 @@
         <v>21.5</v>
       </c>
       <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="D84" s="2">
+        <v>174</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
@@ -1756,7 +1784,9 @@
         <v>25</v>
       </c>
       <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="D85" s="2">
+        <v>176</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
@@ -1766,7 +1796,9 @@
         <v>22.5</v>
       </c>
       <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="D86" s="2">
+        <v>178</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
@@ -1776,7 +1808,9 @@
         <v>27</v>
       </c>
       <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="D87" s="2">
+        <v>180</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
@@ -1786,7 +1820,9 @@
         <v>24.5</v>
       </c>
       <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="D88" s="2">
+        <v>182</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
@@ -1796,7 +1832,9 @@
         <v>26.5</v>
       </c>
       <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
+      <c r="D89" s="2">
+        <v>184</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
@@ -1806,7 +1844,9 @@
         <v>28</v>
       </c>
       <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
+      <c r="D90" s="2">
+        <v>186</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
@@ -1816,7 +1856,9 @@
         <v>29</v>
       </c>
       <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
+      <c r="D91" s="2">
+        <v>188</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
@@ -1826,7 +1868,9 @@
         <v>24</v>
       </c>
       <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
+      <c r="D92" s="2">
+        <v>190</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
@@ -1836,7 +1880,9 @@
         <v>30.5</v>
       </c>
       <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
+      <c r="D93" s="2">
+        <v>192</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
@@ -1846,7 +1892,9 @@
         <v>25</v>
       </c>
       <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
+      <c r="D94" s="2">
+        <v>194</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
@@ -1856,7 +1904,9 @@
         <v>28</v>
       </c>
       <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
+      <c r="D95" s="2">
+        <v>196</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
@@ -1866,7 +1916,9 @@
         <v>27</v>
       </c>
       <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
+      <c r="D96" s="2">
+        <v>198</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
@@ -1876,7 +1928,9 @@
         <v>28</v>
       </c>
       <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
+      <c r="D97" s="2">
+        <v>200</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
@@ -1886,7 +1940,9 @@
         <v>22</v>
       </c>
       <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
+      <c r="D98" s="2">
+        <v>202</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
@@ -1896,7 +1952,9 @@
         <v>27.5</v>
       </c>
       <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
+      <c r="D99" s="2">
+        <v>204</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
@@ -1906,7 +1964,9 @@
         <v>25.5</v>
       </c>
       <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
+      <c r="D100" s="2">
+        <v>206</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
@@ -1916,7 +1976,9 @@
         <v>25</v>
       </c>
       <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
+      <c r="D101" s="2">
+        <v>208</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
@@ -1926,7 +1988,9 @@
         <v>27</v>
       </c>
       <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
+      <c r="D102" s="2">
+        <v>210</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
@@ -3450,15 +3514,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009E16EE7F4C537C4ABFA407FB2C41B1C3" ma:contentTypeVersion="14" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="95de28441f96fc3214151cf7c07046a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="24c72473-a6f8-4ab9-b557-03d61fd61282" xmlns:ns3="6cb94949-7264-4e0b-b21a-9bdc50945768" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8da4ea20e3bb0e14e5b3e046fcf53faa" ns2:_="" ns3:_="">
     <xsd:import namespace="24c72473-a6f8-4ab9-b557-03d61fd61282"/>
@@ -3673,15 +3728,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B729CB-E3EA-410E-92DC-A8953CDD05F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{056E0049-3ACE-4B71-AF49-9AE4CDEAFBA2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3698,4 +3754,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37B729CB-E3EA-410E-92DC-A8953CDD05F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>